<commit_message>
Updated rules file for use with FSS data
</commit_message>
<xml_diff>
--- a/sampleRules/rules.xlsx
+++ b/sampleRules/rules.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
   <si>
     <t>FieldName</t>
   </si>
@@ -30,27 +28,12 @@
     <t>ValidationRegExp</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Height-inches</t>
-  </si>
-  <si>
-    <t>Weight-pounds</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>[0-9]{1,3}</t>
-  </si>
-  <si>
     <t>StandardPseudonym</t>
   </si>
   <si>
@@ -60,7 +43,34 @@
     <t>RemoveField</t>
   </si>
   <si>
-    <t>Spouse</t>
+    <t>EstablishmentName</t>
+  </si>
+  <si>
+    <t>CPH</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Producer Name</t>
+  </si>
+  <si>
+    <t>Producer Address1</t>
+  </si>
+  <si>
+    <t>Producer Address2</t>
+  </si>
+  <si>
+    <t>Producer Postcode</t>
+  </si>
+  <si>
+    <t>Producer Email</t>
+  </si>
+  <si>
+    <t>ProducerName</t>
+  </si>
+  <si>
+    <t>VetName</t>
   </si>
 </sst>
 </file>
@@ -399,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -420,13 +430,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -440,139 +450,206 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>